<commit_message>
done revisi bab2 sama halaman
</commit_message>
<xml_diff>
--- a/STUDI KASUS.xlsx
+++ b/STUDI KASUS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNDIPA\Semester 7\Skripsi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNDIPA\Semester 7\Skripsi\Format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA90620-32F8-4147-B1D3-3ACB645050BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DFACD0-E13D-4F26-AADE-849989DC4311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{901D0503-6946-40CA-8D36-37B156763246}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="229">
   <si>
     <t xml:space="preserve">Biaya </t>
   </si>
@@ -239,9 +239,6 @@
   </si>
   <si>
     <t>Ibadah</t>
-  </si>
-  <si>
-    <t>Prabayar</t>
   </si>
   <si>
     <t>Pada Waktu Sewa</t>
@@ -521,9 +518,6 @@
     <t>Token air</t>
   </si>
   <si>
-    <t>Prabayar (pulsa)</t>
-  </si>
-  <si>
     <t>Jalan kaki</t>
   </si>
   <si>
@@ -735,6 +729,12 @@
   </si>
   <si>
     <t>Ranking</t>
+  </si>
+  <si>
+    <t>&lt;=1</t>
+  </si>
+  <si>
+    <t>kursi</t>
   </si>
 </sst>
 </file>
@@ -850,7 +850,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1228,28 +1238,28 @@
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="12" t="s">
         <v>84</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>85</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>42</v>
@@ -1264,13 +1274,13 @@
         <v>4</v>
       </c>
       <c r="M2" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="N2" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
@@ -1278,43 +1288,43 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>98</v>
-      </c>
       <c r="H3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="K3" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="J3" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>107</v>
-      </c>
       <c r="M3" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N3" s="9" t="s">
         <v>60</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
@@ -1322,43 +1332,43 @@
         <v>2</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>97</v>
-      </c>
       <c r="G4" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L4" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="O4" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
@@ -1366,38 +1376,38 @@
         <v>3</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L5" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="O5" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="72" x14ac:dyDescent="0.3">
@@ -1405,46 +1415,46 @@
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="N6" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="N6" s="9" t="s">
-        <v>126</v>
-      </c>
       <c r="O6" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="72" x14ac:dyDescent="0.3">
@@ -1452,46 +1462,46 @@
         <v>5</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="F7" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="I7" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="G7" s="8" t="s">
+      <c r="J7" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="K7" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>101</v>
-      </c>
       <c r="L7" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="O7" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
@@ -1499,46 +1509,46 @@
         <v>6</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="E8" s="14" t="s">
+      <c r="F8" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G8" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="G8" s="8" t="s">
+      <c r="H8" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="K8" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>133</v>
-      </c>
       <c r="L8" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="N8" t="s">
+        <v>117</v>
+      </c>
+      <c r="O8" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="N8" t="s">
-        <v>118</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -2174,7 +2184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB87EEF9-7F2E-4545-9951-0F532151B120}">
   <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="117" workbookViewId="0">
+    <sheetView zoomScale="117" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -2284,7 +2294,7 @@
         <v>11</v>
       </c>
       <c r="U4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -2350,7 +2360,7 @@
         <v>2</v>
       </c>
       <c r="U6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -2446,7 +2456,7 @@
         <v>5</v>
       </c>
       <c r="U9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
@@ -2461,7 +2471,7 @@
         <v>27</v>
       </c>
       <c r="U10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
@@ -2500,7 +2510,7 @@
         <v>43</v>
       </c>
       <c r="U11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
@@ -2533,12 +2543,12 @@
         <v>11</v>
       </c>
       <c r="U12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -2550,53 +2560,53 @@
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="O13">
         <v>1</v>
       </c>
       <c r="R13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S13">
         <v>1</v>
       </c>
       <c r="U13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G14">
         <v>2</v>
       </c>
       <c r="J14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K14">
         <v>2</v>
       </c>
       <c r="N14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="O14">
         <v>2</v>
       </c>
       <c r="R14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="S14">
         <v>2</v>
       </c>
       <c r="U14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="F15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G15">
         <v>3</v>
@@ -2608,19 +2618,19 @@
         <v>3</v>
       </c>
       <c r="N15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O15">
         <v>3</v>
       </c>
       <c r="R15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S15">
         <v>3</v>
       </c>
       <c r="U15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
@@ -2631,7 +2641,7 @@
         <v>36</v>
       </c>
       <c r="F16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G16">
         <v>4</v>
@@ -2643,13 +2653,13 @@
         <v>4</v>
       </c>
       <c r="R16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S16">
         <v>4</v>
       </c>
       <c r="U16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
@@ -2663,19 +2673,19 @@
         <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G17">
         <v>5</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K17">
         <v>5</v>
       </c>
       <c r="U17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
@@ -2695,7 +2705,7 @@
         <v>42</v>
       </c>
       <c r="U18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
@@ -2726,7 +2736,7 @@
         <v>44</v>
       </c>
       <c r="N20" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="O20">
         <v>1</v>
@@ -2755,7 +2765,7 @@
         <v>5</v>
       </c>
       <c r="N21" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="O21">
         <v>2</v>
@@ -2784,7 +2794,7 @@
         <v>11</v>
       </c>
       <c r="N22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O22">
         <v>3</v>
@@ -2906,8 +2916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BA1C62-8752-4999-BB16-F79297149C3E}">
   <dimension ref="A1:U112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="88" workbookViewId="0">
-      <selection activeCell="F116" sqref="F116"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="88" workbookViewId="0">
+      <selection activeCell="K117" sqref="K117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2929,16 +2939,22 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="U1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>196</v>
+      </c>
       <c r="U2" t="s">
         <v>64</v>
       </c>
@@ -2998,7 +3014,7 @@
         <v>11</v>
       </c>
       <c r="U4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -3020,8 +3036,8 @@
       <c r="K5">
         <v>1</v>
       </c>
-      <c r="N5">
-        <v>1</v>
+      <c r="N5" t="s">
+        <v>227</v>
       </c>
       <c r="O5">
         <v>1</v>
@@ -3038,7 +3054,7 @@
         <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G6">
         <v>2</v>
@@ -3056,7 +3072,7 @@
         <v>2</v>
       </c>
       <c r="U6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -3067,7 +3083,7 @@
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G7">
         <v>3</v>
@@ -3093,7 +3109,7 @@
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G8">
         <v>4</v>
@@ -3109,9 +3125,6 @@
       </c>
       <c r="O8">
         <v>4</v>
-      </c>
-      <c r="U8" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -3139,9 +3152,6 @@
       <c r="O9">
         <v>5</v>
       </c>
-      <c r="U9" t="s">
-        <v>135</v>
-      </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
@@ -3150,9 +3160,6 @@
       <c r="B10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="U10" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
@@ -3185,9 +3192,6 @@
       <c r="R11" t="s">
         <v>43</v>
       </c>
-      <c r="U11" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
@@ -3220,14 +3224,11 @@
       <c r="S12" t="s">
         <v>11</v>
       </c>
-      <c r="U12" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B13" s="15"/>
       <c r="F13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -3239,58 +3240,52 @@
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="O13">
         <v>1</v>
       </c>
       <c r="R13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S13">
         <v>1</v>
-      </c>
-      <c r="U13" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B14" s="15"/>
       <c r="F14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G14">
         <v>2</v>
       </c>
       <c r="J14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K14">
         <v>2</v>
       </c>
       <c r="N14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="O14">
         <v>2</v>
       </c>
       <c r="R14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="S14">
         <v>2</v>
       </c>
-      <c r="U14" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B15" s="15"/>
       <c r="F15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G15">
         <v>3</v>
@@ -3302,26 +3297,23 @@
         <v>3</v>
       </c>
       <c r="N15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O15">
         <v>3</v>
       </c>
       <c r="R15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S15">
         <v>3</v>
-      </c>
-      <c r="U15" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
       <c r="B16" s="15"/>
       <c r="F16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G16">
         <v>4</v>
@@ -3332,40 +3324,28 @@
       <c r="K16">
         <v>4</v>
       </c>
-      <c r="R16" t="s">
-        <v>72</v>
-      </c>
-      <c r="S16">
-        <v>4</v>
-      </c>
-      <c r="U16" t="s">
-        <v>136</v>
-      </c>
     </row>
     <row r="17" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G17">
         <v>5</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K17">
         <v>5</v>
-      </c>
-      <c r="U17" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
@@ -3373,7 +3353,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C18" s="15">
         <f>Ressponden!B2</f>
@@ -3386,7 +3366,7 @@
         <v>42</v>
       </c>
       <c r="U18" t="s">
-        <v>140</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
@@ -3394,7 +3374,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C19" s="15">
         <f>Ressponden!B3</f>
@@ -3406,23 +3386,29 @@
       <c r="O19" t="s">
         <v>11</v>
       </c>
+      <c r="U19" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C20" s="15">
         <f>Ressponden!B4</f>
         <v>10.6</v>
       </c>
       <c r="N20" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="O20">
         <v>1</v>
+      </c>
+      <c r="U20" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
@@ -3430,7 +3416,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C21" s="15">
         <f>Ressponden!B5</f>
@@ -3449,10 +3435,13 @@
         <v>5</v>
       </c>
       <c r="N21" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="O21">
         <v>2</v>
+      </c>
+      <c r="U21" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
@@ -3460,7 +3449,7 @@
         <v>23</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C22" s="15">
         <f>Ressponden!B6</f>
@@ -3479,10 +3468,13 @@
         <v>11</v>
       </c>
       <c r="N22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O22">
         <v>3</v>
+      </c>
+      <c r="U22" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
@@ -3490,7 +3482,7 @@
         <v>24</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C23" s="15">
         <f>Ressponden!B7</f>
@@ -3508,13 +3500,16 @@
       <c r="K23">
         <v>1</v>
       </c>
+      <c r="U23" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C24" s="15">
         <f>Ressponden!B8</f>
@@ -3532,13 +3527,16 @@
       <c r="K24">
         <v>2</v>
       </c>
+      <c r="U24" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C25" s="15">
         <f>Ressponden!B9</f>
@@ -3556,13 +3554,16 @@
       <c r="K25">
         <v>3</v>
       </c>
+      <c r="U25" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C26" s="15">
         <f>Ressponden!B10</f>
@@ -3580,13 +3581,16 @@
       <c r="K26">
         <v>4</v>
       </c>
+      <c r="U26" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C27" s="15">
         <f>Ressponden!B11</f>
@@ -3603,6 +3607,9 @@
       </c>
       <c r="K27">
         <v>5</v>
+      </c>
+      <c r="U27" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.3">
@@ -3612,18 +3619,21 @@
         <f>Ressponden!B12</f>
         <v>100</v>
       </c>
+      <c r="U28" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
@@ -3708,7 +3718,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
@@ -3716,22 +3726,22 @@
     </row>
     <row r="48" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="16" t="s">
-        <v>79</v>
-      </c>
       <c r="C48" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E48" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="D48" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E48" s="16" t="s">
+      <c r="F48" s="16" t="s">
         <v>146</v>
-      </c>
-      <c r="F48" s="16" t="s">
-        <v>147</v>
       </c>
       <c r="G48" s="16" t="s">
         <v>4</v>
@@ -3757,37 +3767,37 @@
         <v>1</v>
       </c>
       <c r="B49" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="C49" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="D49" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="F49" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="D49" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="E49" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="F49" s="12" t="s">
+      <c r="G49" s="12" t="s">
         <v>150</v>
-      </c>
-      <c r="G49" s="12" t="s">
-        <v>151</v>
       </c>
       <c r="H49" s="12" t="s">
         <v>63</v>
       </c>
       <c r="I49" s="12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J49" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K49" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L49" s="12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
@@ -3795,37 +3805,37 @@
         <v>2</v>
       </c>
       <c r="B50" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="F50" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="C50" s="14" t="s">
-        <v>205</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="F50" s="12" t="s">
+      <c r="G50" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="H50" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="G50" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="H50" s="12" t="s">
+      <c r="I50" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="J50" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="I50" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="J50" s="12" t="s">
+      <c r="K50" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="L50" s="12" t="s">
         <v>156</v>
-      </c>
-      <c r="K50" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="L50" s="12" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
@@ -3833,204 +3843,204 @@
         <v>3</v>
       </c>
       <c r="B51" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="F51" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="C51" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="F51" s="12" t="s">
-        <v>161</v>
-      </c>
       <c r="G51" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H51" s="12" t="s">
         <v>63</v>
       </c>
       <c r="I51" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="J51" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="K51" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="L51" s="12" t="s">
         <v>169</v>
-      </c>
-      <c r="J51" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="K51" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="L51" s="12" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>172</v>
-      </c>
-      <c r="B56" t="s">
-        <v>198</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="A56" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G56" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H56" t="s">
+      <c r="H56" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I56" t="s">
+      <c r="I56" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="J56" t="s">
+      <c r="J56" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="K56" t="s">
+      <c r="K56" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="L56" t="s">
+      <c r="L56" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>195</v>
-      </c>
-      <c r="B57" t="s">
-        <v>199</v>
+      <c r="A57" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>197</v>
       </c>
       <c r="C57" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="F57" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="D57" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="F57" s="12" t="s">
+      <c r="G57" s="12" t="s">
         <v>150</v>
-      </c>
-      <c r="G57" s="12" t="s">
-        <v>151</v>
       </c>
       <c r="H57" s="12" t="s">
         <v>63</v>
       </c>
       <c r="I57" s="12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J57" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K57" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L57" s="12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>196</v>
-      </c>
-      <c r="B58" t="s">
-        <v>200</v>
+      <c r="A58" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>198</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E58" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="F58" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="G58" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="H58" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="I58" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="J58" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="K58" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="L58" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A59" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="F59" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="G59" s="12" t="s">
         <v>164</v>
-      </c>
-      <c r="F58" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="G58" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="H58" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="I58" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="J58" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="K58" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="L58" s="12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>197</v>
-      </c>
-      <c r="B59" t="s">
-        <v>201</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="E59" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="F59" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="G59" s="12" t="s">
-        <v>166</v>
       </c>
       <c r="H59" s="12" t="s">
         <v>63</v>
       </c>
       <c r="I59" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="J59" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="K59" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="L59" s="12" t="s">
         <v>169</v>
-      </c>
-      <c r="J59" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="K59" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="L59" s="12" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B65" s="9" t="s">
         <v>19</v>
@@ -4065,7 +4075,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B66" s="9">
         <v>4</v>
@@ -4100,7 +4110,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B67" s="9">
         <v>2</v>
@@ -4135,7 +4145,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B68" s="9">
         <v>2</v>
@@ -4170,37 +4180,37 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="18" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>213</v>
+      </c>
+      <c r="E73" t="s">
+        <v>214</v>
+      </c>
+      <c r="I73" t="s">
         <v>215</v>
-      </c>
-      <c r="E73" t="s">
-        <v>216</v>
-      </c>
-      <c r="I73" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B74">
         <f>2/B66</f>
         <v>0.5</v>
       </c>
       <c r="E74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F74">
         <f>C66/4</f>
         <v>1</v>
       </c>
       <c r="I74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J74">
         <f>D66/4</f>
@@ -4209,78 +4219,78 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B75">
-        <f t="shared" ref="B75:B76" si="0">2/B67</f>
+        <f>2/B67</f>
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F75">
-        <f t="shared" ref="F75:F76" si="1">C67/4</f>
+        <f>C67/4</f>
         <v>0.75</v>
       </c>
       <c r="I75" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J75">
-        <f t="shared" ref="J75:J76" si="2">D67/4</f>
+        <f>D67/4</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B76">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B76" si="0">2/B68</f>
         <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F76">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F76" si="1">C68/4</f>
         <v>1</v>
       </c>
       <c r="I76" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J76">
-        <f t="shared" si="2"/>
+        <f>D68/4</f>
         <v>0.75</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
+        <v>216</v>
+      </c>
+      <c r="E79" t="s">
+        <v>217</v>
+      </c>
+      <c r="I79" t="s">
         <v>218</v>
-      </c>
-      <c r="E79" t="s">
-        <v>219</v>
-      </c>
-      <c r="I79" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B80">
         <f>3/E66</f>
         <v>0.75</v>
       </c>
       <c r="E80" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F80">
         <f>F66/5</f>
         <v>1</v>
       </c>
       <c r="I80" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J80">
         <f>3/G66</f>
@@ -4289,78 +4299,78 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B81">
-        <f t="shared" ref="B81:B82" si="3">3/E67</f>
+        <f>3/E67</f>
         <v>0.75</v>
       </c>
       <c r="E81" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F81">
-        <f t="shared" ref="F81:F82" si="4">F67/5</f>
+        <f>F67/5</f>
         <v>0.8</v>
       </c>
       <c r="I81" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J81">
-        <f t="shared" ref="J81:J82" si="5">3/G67</f>
+        <f>3/G67</f>
         <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B82">
-        <f t="shared" si="3"/>
+        <f>3/E68</f>
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F82">
-        <f t="shared" si="4"/>
+        <f>F68/5</f>
         <v>0.6</v>
       </c>
       <c r="I82" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J82">
-        <f t="shared" si="5"/>
+        <f>3/G68</f>
         <v>0.6</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
+        <v>219</v>
+      </c>
+      <c r="E85" t="s">
+        <v>220</v>
+      </c>
+      <c r="I85" t="s">
         <v>221</v>
-      </c>
-      <c r="E85" t="s">
-        <v>222</v>
-      </c>
-      <c r="I85" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B86">
         <f>H66/4</f>
         <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F86" s="19">
         <f>I66/3</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="I86" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J86" s="19">
         <f>J66/3</f>
@@ -4369,21 +4379,21 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B87">
-        <f t="shared" ref="B87:B88" si="6">H67/4</f>
+        <f>H67/4</f>
         <v>0.75</v>
       </c>
       <c r="E87" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F87" s="19">
         <f>I67/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="I87" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J87" s="19">
         <f>J67/3</f>
@@ -4392,35 +4402,35 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B88">
-        <f t="shared" si="6"/>
+        <f>H68/4</f>
         <v>1</v>
       </c>
       <c r="E88" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F88">
-        <f t="shared" ref="F87:F88" si="7">I68/3</f>
+        <f>I68/3</f>
         <v>1</v>
       </c>
       <c r="I88" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J88">
-        <f t="shared" ref="J87:J88" si="8">J68/3</f>
+        <f t="shared" ref="J88" si="2">J68/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E91" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E92" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F92" s="19">
         <f>K66/3</f>
@@ -4429,7 +4439,7 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E93" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F93" s="19">
         <f>K67/3</f>
@@ -4438,21 +4448,21 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E94" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F94">
-        <f t="shared" ref="F93:F94" si="9">K68/3</f>
+        <f t="shared" ref="F94" si="3">K68/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B100" s="9" t="s">
         <v>19</v>
@@ -4487,7 +4497,7 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101" s="9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B101" s="9">
         <f>B74</f>
@@ -4532,34 +4542,34 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B102" s="9">
-        <f t="shared" ref="B102:B103" si="10">B75</f>
+        <f t="shared" ref="B102:B103" si="4">B75</f>
         <v>1</v>
       </c>
       <c r="C102" s="9">
-        <f t="shared" ref="C102:C103" si="11">F75</f>
+        <f t="shared" ref="C102:C103" si="5">F75</f>
         <v>0.75</v>
       </c>
       <c r="D102" s="9">
-        <f t="shared" ref="D102:D103" si="12">J75</f>
+        <f t="shared" ref="D102:D103" si="6">J75</f>
         <v>0.5</v>
       </c>
       <c r="E102" s="9">
-        <f t="shared" ref="E102:E103" si="13">B81</f>
+        <f t="shared" ref="E102:E103" si="7">B81</f>
         <v>0.75</v>
       </c>
       <c r="F102" s="9">
-        <f t="shared" ref="F102:F103" si="14">F81</f>
+        <f t="shared" ref="F102:F103" si="8">F81</f>
         <v>0.8</v>
       </c>
       <c r="G102" s="9">
-        <f t="shared" ref="G102:G103" si="15">J81</f>
+        <f t="shared" ref="G102:G103" si="9">J81</f>
         <v>1</v>
       </c>
       <c r="H102" s="9">
-        <f t="shared" ref="H102:H103" si="16">B87</f>
+        <f t="shared" ref="H102:H103" si="10">B87</f>
         <v>0.75</v>
       </c>
       <c r="I102" s="20">
@@ -4577,57 +4587,57 @@
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B103" s="9">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="C103" s="9">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="D103" s="9">
+        <f t="shared" si="6"/>
+        <v>0.75</v>
+      </c>
+      <c r="E103" s="9">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="F103" s="9">
+        <f t="shared" si="8"/>
+        <v>0.6</v>
+      </c>
+      <c r="G103" s="9">
+        <f t="shared" si="9"/>
+        <v>0.6</v>
+      </c>
+      <c r="H103" s="9">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="C103" s="9">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="D103" s="9">
-        <f t="shared" si="12"/>
-        <v>0.75</v>
-      </c>
-      <c r="E103" s="9">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="F103" s="9">
-        <f t="shared" si="14"/>
-        <v>0.6</v>
-      </c>
-      <c r="G103" s="9">
-        <f t="shared" si="15"/>
-        <v>0.6</v>
-      </c>
-      <c r="H103" s="9">
-        <f t="shared" si="16"/>
-        <v>1</v>
-      </c>
       <c r="I103" s="9">
-        <f t="shared" ref="I102:I103" si="17">F88</f>
+        <f t="shared" ref="I103" si="11">F88</f>
         <v>1</v>
       </c>
       <c r="J103" s="9">
-        <f t="shared" ref="J102:J103" si="18">J88</f>
+        <f t="shared" ref="J103" si="12">J88</f>
         <v>1</v>
       </c>
       <c r="K103" s="9">
-        <f t="shared" ref="K102:K103" si="19">F94</f>
+        <f t="shared" ref="K103" si="13">F94</f>
         <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B109" s="9" t="s">
         <v>19</v>
@@ -4660,15 +4670,15 @@
         <v>28</v>
       </c>
       <c r="L109" s="9" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M109" s="9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" s="9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B110" s="9">
         <f>B101*C18</f>
@@ -4721,7 +4731,7 @@
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B111" s="9">
         <f>B102*C18</f>
@@ -4768,13 +4778,13 @@
         <v>73.543333333333337</v>
       </c>
       <c r="M111" s="9">
-        <f t="shared" ref="M111:M112" si="20">RANK(L111, $L$110:$L$112, 0)</f>
+        <f t="shared" ref="M111:M112" si="14">RANK(L111, $L$110:$L$112, 0)</f>
         <v>3</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B112" s="9">
         <f>B103*C18</f>
@@ -4821,17 +4831,20 @@
         <v>88.79</v>
       </c>
       <c r="M112" s="9">
-        <f t="shared" si="20"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="K49:K51">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+  <conditionalFormatting sqref="K49">
+    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K50">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K57:K58">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4841,8 +4854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BDD87DC-8644-42C8-A7E5-56F463ADE935}">
   <dimension ref="A1:U112"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" zoomScale="88" workbookViewId="0">
-      <selection activeCell="N71" sqref="N71"/>
+    <sheetView topLeftCell="A93" zoomScale="88" workbookViewId="0">
+      <selection activeCell="G101" sqref="G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4864,10 +4877,10 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="U1" t="s">
         <v>40</v>
@@ -4933,7 +4946,7 @@
         <v>11</v>
       </c>
       <c r="U4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -4973,7 +4986,7 @@
         <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G6">
         <v>2</v>
@@ -4991,7 +5004,7 @@
         <v>2</v>
       </c>
       <c r="U6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -5002,7 +5015,7 @@
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G7">
         <v>3</v>
@@ -5028,7 +5041,7 @@
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G8">
         <v>4</v>
@@ -5075,7 +5088,7 @@
         <v>5</v>
       </c>
       <c r="U9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
@@ -5086,7 +5099,7 @@
         <v>7</v>
       </c>
       <c r="U10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
@@ -5121,7 +5134,7 @@
         <v>43</v>
       </c>
       <c r="U11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
@@ -5156,13 +5169,13 @@
         <v>11</v>
       </c>
       <c r="U12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B13" s="15"/>
       <c r="F13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -5174,58 +5187,58 @@
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="O13">
         <v>1</v>
       </c>
       <c r="R13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S13">
         <v>1</v>
       </c>
       <c r="U13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B14" s="15"/>
       <c r="F14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G14">
         <v>2</v>
       </c>
       <c r="J14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K14">
         <v>2</v>
       </c>
       <c r="N14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="O14">
         <v>2</v>
       </c>
       <c r="R14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="S14">
         <v>2</v>
       </c>
       <c r="U14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B15" s="15"/>
       <c r="F15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G15">
         <v>3</v>
@@ -5237,26 +5250,26 @@
         <v>3</v>
       </c>
       <c r="N15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O15">
         <v>3</v>
       </c>
       <c r="R15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S15">
         <v>3</v>
       </c>
       <c r="U15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
       <c r="B16" s="15"/>
       <c r="F16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G16">
         <v>4</v>
@@ -5268,39 +5281,39 @@
         <v>4</v>
       </c>
       <c r="R16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S16">
         <v>4</v>
       </c>
       <c r="U16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G17">
         <v>5</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K17">
         <v>5</v>
       </c>
       <c r="U17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
@@ -5308,7 +5321,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C18" s="15">
         <f>Ressponden!B2</f>
@@ -5321,7 +5334,7 @@
         <v>42</v>
       </c>
       <c r="U18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
@@ -5329,7 +5342,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C19" s="15">
         <f>Ressponden!B3</f>
@@ -5347,14 +5360,14 @@
         <v>21</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C20" s="15">
         <f>Ressponden!B4</f>
         <v>10.6</v>
       </c>
       <c r="N20" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="O20">
         <v>1</v>
@@ -5365,7 +5378,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C21" s="15">
         <f>Ressponden!B5</f>
@@ -5384,7 +5397,7 @@
         <v>5</v>
       </c>
       <c r="N21" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="O21">
         <v>2</v>
@@ -5395,7 +5408,7 @@
         <v>23</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C22" s="15">
         <f>Ressponden!B6</f>
@@ -5414,7 +5427,7 @@
         <v>11</v>
       </c>
       <c r="N22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O22">
         <v>3</v>
@@ -5425,7 +5438,7 @@
         <v>24</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C23" s="15">
         <f>Ressponden!B7</f>
@@ -5449,7 +5462,7 @@
         <v>25</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C24" s="15">
         <f>Ressponden!B8</f>
@@ -5473,7 +5486,7 @@
         <v>26</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C25" s="15">
         <f>Ressponden!B9</f>
@@ -5497,7 +5510,7 @@
         <v>27</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C26" s="15">
         <f>Ressponden!B10</f>
@@ -5521,7 +5534,7 @@
         <v>28</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C27" s="15">
         <f>Ressponden!B11</f>
@@ -5550,15 +5563,15 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
@@ -5643,7 +5656,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
@@ -5651,22 +5664,22 @@
     </row>
     <row r="48" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="16" t="s">
-        <v>79</v>
-      </c>
       <c r="C48" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E48" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="D48" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E48" s="16" t="s">
+      <c r="F48" s="16" t="s">
         <v>146</v>
-      </c>
-      <c r="F48" s="16" t="s">
-        <v>147</v>
       </c>
       <c r="G48" s="16" t="s">
         <v>4</v>
@@ -5737,15 +5750,15 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C56" s="9" t="s">
         <v>19</v>
@@ -5780,7 +5793,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B57" s="9"/>
       <c r="C57" s="12"/>
@@ -5796,7 +5809,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B58" s="9"/>
       <c r="C58" s="14"/>
@@ -5812,7 +5825,7 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B59" s="9"/>
       <c r="C59" s="12"/>
@@ -5828,12 +5841,12 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B65" s="9" t="s">
         <v>19</v>
@@ -5868,7 +5881,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
@@ -5883,7 +5896,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
@@ -5898,7 +5911,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
@@ -5913,37 +5926,37 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="18" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>213</v>
+      </c>
+      <c r="E73" t="s">
+        <v>214</v>
+      </c>
+      <c r="I73" t="s">
         <v>215</v>
-      </c>
-      <c r="E73" t="s">
-        <v>216</v>
-      </c>
-      <c r="I73" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B74" t="e">
         <f>2/B66</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F74">
         <f>C66/4</f>
         <v>0</v>
       </c>
       <c r="I74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J74">
         <f>D66/4</f>
@@ -5952,21 +5965,21 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B75" t="e">
         <f t="shared" ref="B75:B76" si="0">2/B67</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E75" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F75">
         <f t="shared" ref="F75:F76" si="1">C67/4</f>
         <v>0</v>
       </c>
       <c r="I75" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J75">
         <f t="shared" ref="J75:J76" si="2">D67/4</f>
@@ -5975,21 +5988,21 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B76" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E76" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F76">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I76" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J76">
         <f t="shared" si="2"/>
@@ -5998,32 +6011,32 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
+        <v>216</v>
+      </c>
+      <c r="E79" t="s">
+        <v>217</v>
+      </c>
+      <c r="I79" t="s">
         <v>218</v>
-      </c>
-      <c r="E79" t="s">
-        <v>219</v>
-      </c>
-      <c r="I79" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B80" t="e">
         <f>3/E66</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E80" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F80">
         <f>F66/5</f>
         <v>0</v>
       </c>
       <c r="I80" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J80" t="e">
         <f>3/G66</f>
@@ -6032,21 +6045,21 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B81" t="e">
         <f t="shared" ref="B81:B82" si="3">3/E67</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E81" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F81">
         <f t="shared" ref="F81:F82" si="4">F67/5</f>
         <v>0</v>
       </c>
       <c r="I81" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J81" t="e">
         <f t="shared" ref="J81:J82" si="5">3/G67</f>
@@ -6055,21 +6068,21 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B82" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E82" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F82">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I82" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J82" t="e">
         <f t="shared" si="5"/>
@@ -6078,32 +6091,32 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
+        <v>219</v>
+      </c>
+      <c r="E85" t="s">
+        <v>220</v>
+      </c>
+      <c r="I85" t="s">
         <v>221</v>
-      </c>
-      <c r="E85" t="s">
-        <v>222</v>
-      </c>
-      <c r="I85" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B86">
         <f>H66/4</f>
         <v>0</v>
       </c>
       <c r="E86" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F86" s="19">
         <f>I66/3</f>
         <v>0</v>
       </c>
       <c r="I86" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J86" s="19">
         <f>J66/3</f>
@@ -6112,21 +6125,21 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B87">
         <f t="shared" ref="B87:B88" si="6">H67/4</f>
         <v>0</v>
       </c>
       <c r="E87" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F87" s="19">
         <f>I67/3</f>
         <v>0</v>
       </c>
       <c r="I87" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J87" s="19">
         <f>J67/3</f>
@@ -6135,21 +6148,21 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B88">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E88" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F88">
-        <f t="shared" ref="F88:F89" si="7">I68/3</f>
+        <f t="shared" ref="F88" si="7">I68/3</f>
         <v>0</v>
       </c>
       <c r="I88" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J88">
         <f t="shared" ref="J88" si="8">J68/3</f>
@@ -6158,12 +6171,12 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E91" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E92" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F92" s="19">
         <f>K66/3</f>
@@ -6172,7 +6185,7 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E93" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F93" s="19">
         <f>K67/3</f>
@@ -6181,21 +6194,21 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E94" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F94">
-        <f t="shared" ref="F94:F95" si="9">K68/3</f>
+        <f t="shared" ref="F94" si="9">K68/3</f>
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B100" s="9" t="s">
         <v>19</v>
@@ -6230,7 +6243,7 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101" s="9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B101" s="9" t="e">
         <f>B74</f>
@@ -6275,7 +6288,7 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B102" s="9" t="e">
         <f t="shared" ref="B102:B103" si="10">B75</f>
@@ -6320,7 +6333,7 @@
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B103" s="9" t="e">
         <f t="shared" si="10"/>
@@ -6365,12 +6378,12 @@
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B109" s="9" t="s">
         <v>19</v>
@@ -6403,15 +6416,15 @@
         <v>28</v>
       </c>
       <c r="L109" s="9" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M109" s="9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" s="9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B110" s="9" t="e">
         <f>B101*C18</f>
@@ -6464,7 +6477,7 @@
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B111" s="9" t="e">
         <f>B102*C18</f>
@@ -6517,7 +6530,7 @@
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B112" s="9" t="e">
         <f>B103*C18</f>

</xml_diff>

<commit_message>
done revesi bab 2 studi kasus
</commit_message>
<xml_diff>
--- a/STUDI KASUS.xlsx
+++ b/STUDI KASUS.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNDIPA\Semester 7\Skripsi\Format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DFACD0-E13D-4F26-AADE-849989DC4311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31286E0C-D07D-459B-8F4D-439C946F721E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{901D0503-6946-40CA-8D36-37B156763246}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="691" activeTab="4" xr2:uid="{901D0503-6946-40CA-8D36-37B156763246}"/>
   </bookViews>
   <sheets>
     <sheet name="Kost" sheetId="3" r:id="rId1"/>
     <sheet name="Ressponden" sheetId="1" r:id="rId2"/>
     <sheet name="Bobot Kriteria" sheetId="2" r:id="rId3"/>
-    <sheet name="Studi Kasus" sheetId="4" r:id="rId4"/>
-    <sheet name="Hasil Bab 4" sheetId="6" r:id="rId5"/>
+    <sheet name="Studi Kasus for me" sheetId="4" r:id="rId4"/>
+    <sheet name="Studi Kasus for jurnal" sheetId="8" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
+    <sheet name="Hasil Bab 4" sheetId="6" r:id="rId7"/>
+    <sheet name="tumbal" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="302">
   <si>
     <t xml:space="preserve">Biaya </t>
   </si>
@@ -735,6 +738,225 @@
   </si>
   <si>
     <t>kursi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kebersihan </t>
+  </si>
+  <si>
+    <t>Jenis listrik</t>
+  </si>
+  <si>
+    <t>Kebersihan</t>
+  </si>
+  <si>
+    <t>dibersihkan setiap hari</t>
+  </si>
+  <si>
+    <t>dibersihkan seminggu hari</t>
+  </si>
+  <si>
+    <t>dibersihkan sebulan sekali</t>
+  </si>
+  <si>
+    <t>Ukuran Kamar (m²)</t>
+  </si>
+  <si>
+    <t>Kos Kantin Surabaya</t>
+  </si>
+  <si>
+    <t>&gt;Rp.900.000 – Rp.1.300.000</t>
+  </si>
+  <si>
+    <t>Lengkap (Kasur, Lemari, AC, Kamar Mandi Dalam, WiFi, Parkir Luas)</t>
+  </si>
+  <si>
+    <t>Lengkap (dekat tempat makan, ibadah, hiburan)</t>
+  </si>
+  <si>
+    <t>Tidak ada batas jam malam</t>
+  </si>
+  <si>
+    <t>Dibersihkan setiap hari</t>
+  </si>
+  <si>
+    <t>50 meter</t>
+  </si>
+  <si>
+    <t>Amanah Kos</t>
+  </si>
+  <si>
+    <t>Lengkap (dekat tempat makan, warung, ibadah, hiburan)</t>
+  </si>
+  <si>
+    <t>CCTV &amp; Penjaga</t>
+  </si>
+  <si>
+    <t>21.00–22.00</t>
+  </si>
+  <si>
+    <t>Prabayar</t>
+  </si>
+  <si>
+    <t>D’Orange</t>
+  </si>
+  <si>
+    <t>≤Rp.700.000 – Rp.900.000</t>
+  </si>
+  <si>
+    <t>Cukup Lengkap (dekat makan, ibadah, hiburan)</t>
+  </si>
+  <si>
+    <t>23.00–24.00</t>
+  </si>
+  <si>
+    <t>&gt;250 meter – 1 km</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>Kos Janji</t>
+  </si>
+  <si>
+    <t>Cukup Lengkap (Kasur, Lemari, Kipas, KM Dalam)</t>
+  </si>
+  <si>
+    <t>Lengkap (dekat makan, warung, ibadah, hiburan)</t>
+  </si>
+  <si>
+    <t>Tidak ada keamanan</t>
+  </si>
+  <si>
+    <t>Dibersihkan seminggu sekali</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>Kos Faazana</t>
+  </si>
+  <si>
+    <t>Lengkap (Kasur, Lemari, AC, KM Dalam, WiFi, Parkir)</t>
+  </si>
+  <si>
+    <t>Lengkap (dekat makan, ibadah, hiburan)</t>
+  </si>
+  <si>
+    <t>&gt;50 – 250 meter</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>Graha Green</t>
+  </si>
+  <si>
+    <t>Ukuran ruangan</t>
+  </si>
+  <si>
+    <t>50 m</t>
+  </si>
+  <si>
+    <t>&gt;50 -250 m</t>
+  </si>
+  <si>
+    <t>&gt;250 - 1km</t>
+  </si>
+  <si>
+    <t>&gt;1km -2.5 km</t>
+  </si>
+  <si>
+    <t>&lt;= RP.700.000 - Rp. 900.000</t>
+  </si>
+  <si>
+    <t>&gt; RP.900.000 - Rp. 1.300.000</t>
+  </si>
+  <si>
+    <t>&gt; RP.1.300.000 - Rp. 1.600.00</t>
+  </si>
+  <si>
+    <t>&gt; RP.1.600.000 - Rp. 2.000.00</t>
+  </si>
+  <si>
+    <t>Kasur, lemari, kipas</t>
+  </si>
+  <si>
+    <t>Kasur, lemari, kipas/Ac, kamar mandi dalam</t>
+  </si>
+  <si>
+    <t>Kasur, lemari, kipas/Ac, kamar mandi dalam, wifi dan parkir</t>
+  </si>
+  <si>
+    <t>keterangan</t>
+  </si>
+  <si>
+    <t>Sangat tidak lengkap</t>
+  </si>
+  <si>
+    <t>tidak lengkap</t>
+  </si>
+  <si>
+    <t>cukup lengkap</t>
+  </si>
+  <si>
+    <t>lengkap</t>
+  </si>
+  <si>
+    <t>Dekat dengan tempat hiburan</t>
+  </si>
+  <si>
+    <t>dekat dengan tempat makan sama tempat hiburan</t>
+  </si>
+  <si>
+    <t>dekat dengan tempat makan sama tempat hiburan, ibadah</t>
+  </si>
+  <si>
+    <t>dekat dengan tempat makan sama tempat hiburan, warung</t>
+  </si>
+  <si>
+    <t>satpam</t>
+  </si>
+  <si>
+    <t>3x3 m^2</t>
+  </si>
+  <si>
+    <t>3x4m^2</t>
+  </si>
+  <si>
+    <t>4x5m^2</t>
+  </si>
+  <si>
+    <t>5x6^2</t>
+  </si>
+  <si>
+    <t>21:00 - 22:00</t>
+  </si>
+  <si>
+    <t>23:00 - 24:00</t>
+  </si>
+  <si>
+    <t>bebas</t>
+  </si>
+  <si>
+    <t>01:00-02:00</t>
+  </si>
+  <si>
+    <t>C2= Cost: Nilai minimal / Nilai Alternatif Kriteria</t>
+  </si>
+  <si>
+    <t>C7= Cost: Nilai minimal / Nilai Alternatif Kriteria</t>
+  </si>
+  <si>
+    <t>C9= Cost: Nilai minimal / Nilai Alternatif Kriteria</t>
+  </si>
+  <si>
+    <t>CCTV dan satpam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C4= Benefit: Nilai Alternatif Kriteria/ Nilai Maximal  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C6= Benefit: Nilai Alternatif Kriteria/ Nilai Maximal  </t>
   </si>
 </sst>
 </file>
@@ -790,7 +1012,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -846,11 +1068,38 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1638,7 +1887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7917028-436B-4FE2-9CD4-951DC7160D43}">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView zoomScale="118" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="118" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2916,7 +3165,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BA1C62-8752-4999-BB16-F79297149C3E}">
   <dimension ref="A1:U112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="88" workbookViewId="0">
+    <sheetView topLeftCell="A99" zoomScale="88" workbookViewId="0">
       <selection activeCell="K117" sqref="K117"/>
     </sheetView>
   </sheetViews>
@@ -4838,19 +5087,2589 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="K49">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K50">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K57:K58">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6626FB-65A5-4DCB-9E1D-A2FA0EB2B8E1}">
+  <dimension ref="A1:P119"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="99" zoomScaleNormal="123" workbookViewId="0">
+      <selection activeCell="L125" sqref="L125"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" customWidth="1"/>
+    <col min="11" max="11" width="15.77734375" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" customWidth="1"/>
+    <col min="14" max="14" width="18.44140625" customWidth="1"/>
+    <col min="15" max="15" width="22.21875" customWidth="1"/>
+    <col min="16" max="16" width="33.109375" customWidth="1"/>
+    <col min="20" max="20" width="17.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" t="s">
+        <v>196</v>
+      </c>
+      <c r="L4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>267</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="O5" t="s">
+        <v>292</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" t="s">
+        <v>268</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="P6" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>269</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="L7">
+        <v>3</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="P7" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="F8" t="s">
+        <v>270</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="L8">
+        <v>4</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="P8" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" t="s">
+        <v>4</v>
+      </c>
+      <c r="N11" t="s">
+        <v>26</v>
+      </c>
+      <c r="O11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
+      <c r="B12" s="17"/>
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L12" t="s">
+        <v>11</v>
+      </c>
+      <c r="O12" t="s">
+        <v>29</v>
+      </c>
+      <c r="P12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B13" s="15"/>
+      <c r="F13" t="s">
+        <v>271</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="K13" t="s">
+        <v>56</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="O13" t="s">
+        <v>204</v>
+      </c>
+      <c r="P13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B14" s="15"/>
+      <c r="F14" t="s">
+        <v>272</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="K14" t="s">
+        <v>287</v>
+      </c>
+      <c r="L14">
+        <v>2</v>
+      </c>
+      <c r="O14" t="s">
+        <v>205</v>
+      </c>
+      <c r="P14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="F15" t="s">
+        <v>273</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="K15" t="s">
+        <v>58</v>
+      </c>
+      <c r="L15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="9"/>
+      <c r="B16" s="15"/>
+      <c r="F16" t="s">
+        <v>274</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="K16" t="s">
+        <v>299</v>
+      </c>
+      <c r="L16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="C18" s="15">
+        <v>15</v>
+      </c>
+      <c r="N18" t="s">
+        <v>27</v>
+      </c>
+      <c r="O18" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="C19" s="15">
+        <v>20</v>
+      </c>
+      <c r="O19" t="s">
+        <v>29</v>
+      </c>
+      <c r="P19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="C20" s="15">
+        <v>15</v>
+      </c>
+      <c r="O20" t="s">
+        <v>232</v>
+      </c>
+      <c r="P20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21" s="15">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" t="s">
+        <v>24</v>
+      </c>
+      <c r="K21" t="s">
+        <v>266</v>
+      </c>
+      <c r="O21" t="s">
+        <v>233</v>
+      </c>
+      <c r="P21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="C22" s="15">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" t="s">
+        <v>278</v>
+      </c>
+      <c r="H22" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" t="s">
+        <v>29</v>
+      </c>
+      <c r="L22" t="s">
+        <v>11</v>
+      </c>
+      <c r="O22" t="s">
+        <v>234</v>
+      </c>
+      <c r="P22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="C23" s="15">
+        <v>5</v>
+      </c>
+      <c r="F23" t="s">
+        <v>275</v>
+      </c>
+      <c r="G23" t="s">
+        <v>279</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="K23" t="s">
+        <v>288</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="C24" s="15">
+        <v>5</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="K24" t="s">
+        <v>289</v>
+      </c>
+      <c r="L24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C25" s="15">
+        <v>5</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="H25">
+        <v>3</v>
+      </c>
+      <c r="K25" t="s">
+        <v>290</v>
+      </c>
+      <c r="L25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="C26" s="15">
+        <v>15</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="K26" t="s">
+        <v>291</v>
+      </c>
+      <c r="L26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="9"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15">
+        <f>C18+C19+C20+C21+C22+C23+C24+C25+C26</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A36" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A37" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A38" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A39" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A40" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A41" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A47" s="18"/>
+    </row>
+    <row r="48" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F48" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="G48" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H48" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I48" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="J48" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="K48" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="L48" s="16"/>
+      <c r="M48" s="16"/>
+    </row>
+    <row r="49" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H49" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="I49" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="J49" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="K49" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="L49" s="12"/>
+      <c r="M49" s="12"/>
+    </row>
+    <row r="50" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="I50" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="J50" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="K50" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="L50" s="12"/>
+      <c r="M50" s="12"/>
+    </row>
+    <row r="51" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="G51" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="H51" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="I51" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="J51" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="K51" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="L51" s="12"/>
+      <c r="M51" s="12"/>
+    </row>
+    <row r="52" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A52" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="F52" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="H52" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="I52" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="J52" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="K52" s="12" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A53" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="F53" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="G53" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H53" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="I53" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="J53" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="K53" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A54" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="G54" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="H54" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="I54" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="J54" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="K54" s="12" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A56" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G56" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H56" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I56" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J56" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K56" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M56" s="9"/>
+      <c r="N56" s="9"/>
+    </row>
+    <row r="57" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="I57" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="J57" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="K57" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="M57" s="9"/>
+      <c r="N57" s="17"/>
+    </row>
+    <row r="58" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="H58" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="I58" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="J58" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="K58" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="M58" s="9"/>
+      <c r="N58" s="17"/>
+    </row>
+    <row r="59" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="H59" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="I59" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="J59" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="K59" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="M59" s="9"/>
+      <c r="N59" s="17"/>
+    </row>
+    <row r="60" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A60" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="H60" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="I60" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="J60" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="K60" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="M60" s="9"/>
+      <c r="N60" s="17"/>
+    </row>
+    <row r="61" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A61" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H61" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="I61" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="J61" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="K61" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="M61" s="9"/>
+      <c r="N61" s="17"/>
+    </row>
+    <row r="62" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A62" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="H62" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="I62" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="J62" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="K62" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="M62" s="9"/>
+      <c r="N62" s="17"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M63" s="9"/>
+      <c r="N63" s="17"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>207</v>
+      </c>
+      <c r="M64" s="9"/>
+      <c r="N64" s="17"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M65" s="9"/>
+      <c r="N65" s="17"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A66" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H66" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I66" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J66" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K66" s="9"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A67" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B67" s="9">
+        <v>1</v>
+      </c>
+      <c r="C67" s="9">
+        <v>2</v>
+      </c>
+      <c r="D67" s="9">
+        <v>4</v>
+      </c>
+      <c r="E67" s="9">
+        <v>4</v>
+      </c>
+      <c r="F67" s="9">
+        <v>3</v>
+      </c>
+      <c r="G67" s="9">
+        <v>2</v>
+      </c>
+      <c r="H67" s="9">
+        <v>4</v>
+      </c>
+      <c r="I67" s="9">
+        <v>3</v>
+      </c>
+      <c r="J67" s="9">
+        <v>2</v>
+      </c>
+      <c r="K67" s="9"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A68" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B68" s="9">
+        <v>1</v>
+      </c>
+      <c r="C68" s="9">
+        <v>2</v>
+      </c>
+      <c r="D68" s="9">
+        <v>4</v>
+      </c>
+      <c r="E68" s="9">
+        <v>4</v>
+      </c>
+      <c r="F68" s="9">
+        <v>4</v>
+      </c>
+      <c r="G68" s="9">
+        <v>2</v>
+      </c>
+      <c r="H68" s="9">
+        <v>1</v>
+      </c>
+      <c r="I68" s="9">
+        <v>7</v>
+      </c>
+      <c r="J68" s="9">
+        <v>2</v>
+      </c>
+      <c r="K68" s="9"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A69" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B69" s="9">
+        <v>3</v>
+      </c>
+      <c r="C69" s="9">
+        <v>1</v>
+      </c>
+      <c r="D69" s="9">
+        <v>4</v>
+      </c>
+      <c r="E69" s="9">
+        <v>3</v>
+      </c>
+      <c r="F69" s="9">
+        <v>4</v>
+      </c>
+      <c r="G69" s="9">
+        <v>2</v>
+      </c>
+      <c r="H69" s="9">
+        <v>2</v>
+      </c>
+      <c r="I69" s="9">
+        <v>7</v>
+      </c>
+      <c r="J69" s="9">
+        <v>2</v>
+      </c>
+      <c r="K69" s="9"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A70" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="B70" s="9">
+        <v>1</v>
+      </c>
+      <c r="C70" s="9">
+        <v>1</v>
+      </c>
+      <c r="D70" s="9">
+        <v>3</v>
+      </c>
+      <c r="E70" s="9">
+        <v>4</v>
+      </c>
+      <c r="F70" s="9">
+        <v>1</v>
+      </c>
+      <c r="G70" s="9">
+        <v>2</v>
+      </c>
+      <c r="H70" s="9">
+        <v>2</v>
+      </c>
+      <c r="I70" s="9">
+        <v>7</v>
+      </c>
+      <c r="J70" s="9">
+        <v>3</v>
+      </c>
+      <c r="K70" s="9"/>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A71" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="B71" s="9">
+        <v>2</v>
+      </c>
+      <c r="C71" s="9">
+        <v>2</v>
+      </c>
+      <c r="D71" s="9">
+        <v>3</v>
+      </c>
+      <c r="E71" s="9">
+        <v>3</v>
+      </c>
+      <c r="F71" s="9">
+        <v>3</v>
+      </c>
+      <c r="G71" s="9">
+        <v>2</v>
+      </c>
+      <c r="H71" s="9">
+        <v>1</v>
+      </c>
+      <c r="I71" s="9">
+        <v>7</v>
+      </c>
+      <c r="J71" s="9">
+        <v>2</v>
+      </c>
+      <c r="K71" s="9"/>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A72" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="B72" s="9">
+        <v>3</v>
+      </c>
+      <c r="C72" s="9">
+        <v>2</v>
+      </c>
+      <c r="D72" s="9">
+        <v>3</v>
+      </c>
+      <c r="E72" s="9">
+        <v>3</v>
+      </c>
+      <c r="F72" s="9">
+        <v>4</v>
+      </c>
+      <c r="G72" s="9">
+        <v>2</v>
+      </c>
+      <c r="H72" s="9">
+        <v>1</v>
+      </c>
+      <c r="I72" s="9">
+        <v>7</v>
+      </c>
+      <c r="J72" s="9">
+        <v>2</v>
+      </c>
+      <c r="K72" s="9"/>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J73" s="9"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A74" s="18" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>213</v>
+      </c>
+      <c r="E77" t="s">
+        <v>296</v>
+      </c>
+      <c r="J77" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>193</v>
+      </c>
+      <c r="B78">
+        <f t="shared" ref="B78:B83" si="0">1/B67</f>
+        <v>1</v>
+      </c>
+      <c r="E78" t="s">
+        <v>193</v>
+      </c>
+      <c r="F78">
+        <f>1/C67</f>
+        <v>0.5</v>
+      </c>
+      <c r="J78" t="s">
+        <v>193</v>
+      </c>
+      <c r="K78">
+        <f>D67/4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>194</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E79" t="s">
+        <v>194</v>
+      </c>
+      <c r="F79">
+        <f t="shared" ref="F79:F83" si="1">1/C68</f>
+        <v>0.5</v>
+      </c>
+      <c r="J79" t="s">
+        <v>194</v>
+      </c>
+      <c r="K79">
+        <f t="shared" ref="K79:K83" si="2">D68/4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>195</v>
+      </c>
+      <c r="B80" s="19">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E80" t="s">
+        <v>195</v>
+      </c>
+      <c r="F80">
+        <f>1/C69</f>
+        <v>1</v>
+      </c>
+      <c r="J80" t="s">
+        <v>195</v>
+      </c>
+      <c r="K80">
+        <f>D69/4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>253</v>
+      </c>
+      <c r="B81">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E81" t="s">
+        <v>253</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J81" t="s">
+        <v>253</v>
+      </c>
+      <c r="K81">
+        <f>D70/4</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>259</v>
+      </c>
+      <c r="B82">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="E82" t="s">
+        <v>259</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="J82" t="s">
+        <v>259</v>
+      </c>
+      <c r="K82">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>264</v>
+      </c>
+      <c r="B83" s="19">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E83" t="s">
+        <v>264</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="J83" t="s">
+        <v>264</v>
+      </c>
+      <c r="K83">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>300</v>
+      </c>
+      <c r="E85" t="s">
+        <v>217</v>
+      </c>
+      <c r="J85" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>193</v>
+      </c>
+      <c r="B86">
+        <f>E67/4</f>
+        <v>1</v>
+      </c>
+      <c r="E86" t="s">
+        <v>193</v>
+      </c>
+      <c r="F86">
+        <f>F67/4</f>
+        <v>0.75</v>
+      </c>
+      <c r="J86" t="s">
+        <v>193</v>
+      </c>
+      <c r="K86">
+        <f>G67/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>194</v>
+      </c>
+      <c r="B87">
+        <f>E68/4</f>
+        <v>1</v>
+      </c>
+      <c r="E87" t="s">
+        <v>194</v>
+      </c>
+      <c r="F87">
+        <f>F68/4</f>
+        <v>1</v>
+      </c>
+      <c r="J87" t="s">
+        <v>194</v>
+      </c>
+      <c r="K87">
+        <f t="shared" ref="K87:K91" si="3">G68/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>195</v>
+      </c>
+      <c r="B88">
+        <f>E69/4</f>
+        <v>0.75</v>
+      </c>
+      <c r="E88" t="s">
+        <v>195</v>
+      </c>
+      <c r="F88">
+        <f t="shared" ref="F88:F91" si="4">F69/4</f>
+        <v>1</v>
+      </c>
+      <c r="J88" t="s">
+        <v>195</v>
+      </c>
+      <c r="K88">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>253</v>
+      </c>
+      <c r="B89">
+        <f>E70/4</f>
+        <v>1</v>
+      </c>
+      <c r="E89" t="s">
+        <v>253</v>
+      </c>
+      <c r="F89">
+        <f>F70/4</f>
+        <v>0.25</v>
+      </c>
+      <c r="J89" t="s">
+        <v>253</v>
+      </c>
+      <c r="K89">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>259</v>
+      </c>
+      <c r="B90">
+        <f>E71/4</f>
+        <v>0.75</v>
+      </c>
+      <c r="E90" t="s">
+        <v>259</v>
+      </c>
+      <c r="F90">
+        <f>F71/4</f>
+        <v>0.75</v>
+      </c>
+      <c r="J90" t="s">
+        <v>259</v>
+      </c>
+      <c r="K90">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>264</v>
+      </c>
+      <c r="B91">
+        <f t="shared" ref="B91" si="5">E72/4</f>
+        <v>0.75</v>
+      </c>
+      <c r="E91" t="s">
+        <v>264</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J91" t="s">
+        <v>264</v>
+      </c>
+      <c r="K91">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>297</v>
+      </c>
+      <c r="E93" t="s">
+        <v>220</v>
+      </c>
+      <c r="J93" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>193</v>
+      </c>
+      <c r="B94">
+        <f>1/H67</f>
+        <v>0.25</v>
+      </c>
+      <c r="E94" t="s">
+        <v>193</v>
+      </c>
+      <c r="F94" s="19">
+        <f>I67/7</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="G94" s="19"/>
+      <c r="J94" t="s">
+        <v>193</v>
+      </c>
+      <c r="K94" s="23">
+        <f>2/J67</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>194</v>
+      </c>
+      <c r="B95">
+        <f>1/H68</f>
+        <v>1</v>
+      </c>
+      <c r="E95" t="s">
+        <v>194</v>
+      </c>
+      <c r="F95" s="23">
+        <f>I68/7</f>
+        <v>1</v>
+      </c>
+      <c r="G95" s="19"/>
+      <c r="J95" t="s">
+        <v>194</v>
+      </c>
+      <c r="K95" s="23">
+        <f>2/J68</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>195</v>
+      </c>
+      <c r="B96">
+        <f>1/H69</f>
+        <v>0.5</v>
+      </c>
+      <c r="E96" t="s">
+        <v>195</v>
+      </c>
+      <c r="F96" s="23">
+        <f t="shared" ref="F96:F99" si="6">I69/7</f>
+        <v>1</v>
+      </c>
+      <c r="J96" t="s">
+        <v>195</v>
+      </c>
+      <c r="K96" s="23">
+        <f t="shared" ref="K96" si="7">2/J69</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>253</v>
+      </c>
+      <c r="B97">
+        <f>1/H70</f>
+        <v>0.5</v>
+      </c>
+      <c r="E97" t="s">
+        <v>253</v>
+      </c>
+      <c r="F97" s="23">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J97" t="s">
+        <v>253</v>
+      </c>
+      <c r="K97" s="19">
+        <f>2/J70</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>259</v>
+      </c>
+      <c r="B98">
+        <f>1/H71</f>
+        <v>1</v>
+      </c>
+      <c r="E98" t="s">
+        <v>259</v>
+      </c>
+      <c r="F98" s="23">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J98" t="s">
+        <v>259</v>
+      </c>
+      <c r="K98" s="23">
+        <f t="shared" ref="K98:K99" si="8">2/J71</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>264</v>
+      </c>
+      <c r="B99">
+        <f t="shared" ref="B99" si="9">1/H72</f>
+        <v>1</v>
+      </c>
+      <c r="E99" t="s">
+        <v>264</v>
+      </c>
+      <c r="F99" s="23">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J99" t="s">
+        <v>264</v>
+      </c>
+      <c r="K99" s="23">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F100" s="19"/>
+      <c r="K100" s="19"/>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A103" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C103" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D103" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E103" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F103" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G103" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H103" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I103" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J103" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L103" s="9"/>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A104" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B104" s="9">
+        <f>B78</f>
+        <v>1</v>
+      </c>
+      <c r="C104" s="9">
+        <f>F78</f>
+        <v>0.5</v>
+      </c>
+      <c r="D104" s="9">
+        <f>K78</f>
+        <v>1</v>
+      </c>
+      <c r="E104" s="9">
+        <f>B86</f>
+        <v>1</v>
+      </c>
+      <c r="F104" s="9">
+        <f>F86</f>
+        <v>0.75</v>
+      </c>
+      <c r="G104" s="20">
+        <f>K86</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H104" s="9">
+        <f>B94</f>
+        <v>0.25</v>
+      </c>
+      <c r="I104" s="20">
+        <f>F94</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="J104" s="20">
+        <f>K94</f>
+        <v>1</v>
+      </c>
+      <c r="L104" s="20"/>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A105" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B105" s="9">
+        <f>B79</f>
+        <v>1</v>
+      </c>
+      <c r="C105" s="9">
+        <f>F79</f>
+        <v>0.5</v>
+      </c>
+      <c r="D105" s="9">
+        <f>K79</f>
+        <v>1</v>
+      </c>
+      <c r="E105" s="9">
+        <f>B87</f>
+        <v>1</v>
+      </c>
+      <c r="F105" s="9">
+        <f>F87</f>
+        <v>1</v>
+      </c>
+      <c r="G105" s="20">
+        <f>K87</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H105" s="9">
+        <f>B95</f>
+        <v>1</v>
+      </c>
+      <c r="I105" s="20">
+        <f>F95</f>
+        <v>1</v>
+      </c>
+      <c r="J105" s="20">
+        <f>K95</f>
+        <v>1</v>
+      </c>
+      <c r="L105" s="20"/>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A106" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B106" s="20">
+        <f>B80</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C106" s="9">
+        <f>F80</f>
+        <v>1</v>
+      </c>
+      <c r="D106" s="9">
+        <f>K80</f>
+        <v>1</v>
+      </c>
+      <c r="E106" s="9">
+        <f>B88</f>
+        <v>0.75</v>
+      </c>
+      <c r="F106" s="9">
+        <f>F88</f>
+        <v>1</v>
+      </c>
+      <c r="G106" s="20">
+        <f>K88</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H106" s="9">
+        <f>B96</f>
+        <v>0.5</v>
+      </c>
+      <c r="I106" s="9">
+        <f>F96</f>
+        <v>1</v>
+      </c>
+      <c r="J106" s="9">
+        <f>K96</f>
+        <v>1</v>
+      </c>
+      <c r="L106" s="9"/>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A107" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="B107" s="22">
+        <f>B81</f>
+        <v>1</v>
+      </c>
+      <c r="C107" s="9">
+        <f t="shared" ref="C107:C109" si="10">F81</f>
+        <v>1</v>
+      </c>
+      <c r="D107" s="9">
+        <f t="shared" ref="D107:D109" si="11">K81</f>
+        <v>0.75</v>
+      </c>
+      <c r="E107" s="9">
+        <f t="shared" ref="E107:E109" si="12">B89</f>
+        <v>1</v>
+      </c>
+      <c r="F107" s="9">
+        <f t="shared" ref="F107:F109" si="13">F89</f>
+        <v>0.25</v>
+      </c>
+      <c r="G107" s="20">
+        <f t="shared" ref="G107:G109" si="14">K89</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H107" s="9">
+        <f t="shared" ref="H107:H109" si="15">B97</f>
+        <v>0.5</v>
+      </c>
+      <c r="I107" s="9">
+        <f t="shared" ref="I107:I109" si="16">F97</f>
+        <v>1</v>
+      </c>
+      <c r="J107" s="20">
+        <f t="shared" ref="J107:J109" si="17">K97</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K107" s="9"/>
+      <c r="L107" s="9"/>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A108" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="B108" s="20">
+        <f>B82</f>
+        <v>0.5</v>
+      </c>
+      <c r="C108" s="9">
+        <f t="shared" si="10"/>
+        <v>0.5</v>
+      </c>
+      <c r="D108" s="9">
+        <f t="shared" si="11"/>
+        <v>0.75</v>
+      </c>
+      <c r="E108" s="9">
+        <f t="shared" si="12"/>
+        <v>0.75</v>
+      </c>
+      <c r="F108" s="9">
+        <f t="shared" si="13"/>
+        <v>0.75</v>
+      </c>
+      <c r="G108" s="20">
+        <f t="shared" si="14"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H108" s="9">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="I108" s="9">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="J108" s="9">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A109" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="B109" s="20">
+        <f t="shared" ref="B109" si="18">B83</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C109" s="9">
+        <f t="shared" si="10"/>
+        <v>0.5</v>
+      </c>
+      <c r="D109" s="9">
+        <f t="shared" si="11"/>
+        <v>0.75</v>
+      </c>
+      <c r="E109" s="9">
+        <f t="shared" si="12"/>
+        <v>0.75</v>
+      </c>
+      <c r="F109" s="9">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="G109" s="20">
+        <f t="shared" si="14"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H109" s="9">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="I109" s="9">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="J109" s="9">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A113" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="B113" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C113" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D113" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E113" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F113" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G113" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H113" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I113" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J113" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K113" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="L113" s="9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A114" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B114" s="9">
+        <f>B104*C18</f>
+        <v>15</v>
+      </c>
+      <c r="C114" s="9">
+        <f>C104*C19</f>
+        <v>10</v>
+      </c>
+      <c r="D114" s="9">
+        <f>D104*C20</f>
+        <v>15</v>
+      </c>
+      <c r="E114" s="9">
+        <f>E104*C21</f>
+        <v>10</v>
+      </c>
+      <c r="F114" s="9">
+        <f>F104*C22</f>
+        <v>7.5</v>
+      </c>
+      <c r="G114" s="20">
+        <f>G104*C23</f>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="H114" s="9">
+        <f>H104*C24</f>
+        <v>1.25</v>
+      </c>
+      <c r="I114" s="20">
+        <f>I104*C25</f>
+        <v>2.1428571428571428</v>
+      </c>
+      <c r="J114" s="20">
+        <f>J104*C26</f>
+        <v>15</v>
+      </c>
+      <c r="K114" s="20">
+        <f>SUM(B114:J114)</f>
+        <v>79.226190476190482</v>
+      </c>
+      <c r="L114" s="9">
+        <f t="shared" ref="L114:L119" si="19">RANK(K114, $K$114:$K$119, 0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A115" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B115" s="9">
+        <f>B105*C18</f>
+        <v>15</v>
+      </c>
+      <c r="C115" s="9">
+        <f>C105*C19</f>
+        <v>10</v>
+      </c>
+      <c r="D115" s="9">
+        <f>D105*C20</f>
+        <v>15</v>
+      </c>
+      <c r="E115" s="9">
+        <f>E105*C21</f>
+        <v>10</v>
+      </c>
+      <c r="F115" s="9">
+        <f>F105*C22</f>
+        <v>10</v>
+      </c>
+      <c r="G115" s="20">
+        <f>G105*C23</f>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="H115" s="9">
+        <f>H105*C24</f>
+        <v>5</v>
+      </c>
+      <c r="I115" s="9">
+        <f>I105*C25</f>
+        <v>5</v>
+      </c>
+      <c r="J115" s="20">
+        <f>J105*C26</f>
+        <v>15</v>
+      </c>
+      <c r="K115" s="20">
+        <f>SUM(B115:J115)</f>
+        <v>88.333333333333343</v>
+      </c>
+      <c r="L115" s="9">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A116" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B116" s="9">
+        <f>B106*C18</f>
+        <v>5</v>
+      </c>
+      <c r="C116" s="9">
+        <f>C106*C19</f>
+        <v>20</v>
+      </c>
+      <c r="D116" s="9">
+        <f>D106*C20</f>
+        <v>15</v>
+      </c>
+      <c r="E116" s="9">
+        <f>E106*C21</f>
+        <v>7.5</v>
+      </c>
+      <c r="F116" s="9">
+        <f>F106*C22</f>
+        <v>10</v>
+      </c>
+      <c r="G116" s="20">
+        <f>G106*C23</f>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="H116" s="9">
+        <f>H106*C24</f>
+        <v>2.5</v>
+      </c>
+      <c r="I116" s="9">
+        <f>I106*C25</f>
+        <v>5</v>
+      </c>
+      <c r="J116" s="9">
+        <f>J106*C26</f>
+        <v>15</v>
+      </c>
+      <c r="K116" s="20">
+        <f>SUM(B116:J116)</f>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="L116" s="9">
+        <f t="shared" si="19"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A117" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="B117" s="9">
+        <f>B107*C18</f>
+        <v>15</v>
+      </c>
+      <c r="C117" s="9">
+        <f>C107*C19</f>
+        <v>20</v>
+      </c>
+      <c r="D117" s="9">
+        <f>D107*C20</f>
+        <v>11.25</v>
+      </c>
+      <c r="E117" s="9">
+        <f>E107*C21</f>
+        <v>10</v>
+      </c>
+      <c r="F117" s="9">
+        <f>F107*C22</f>
+        <v>2.5</v>
+      </c>
+      <c r="G117" s="20">
+        <f>G107*C23</f>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="H117" s="9">
+        <f>H107*C24</f>
+        <v>2.5</v>
+      </c>
+      <c r="I117" s="9">
+        <f>I107*C25</f>
+        <v>5</v>
+      </c>
+      <c r="J117" s="20">
+        <f>J107*C26</f>
+        <v>10</v>
+      </c>
+      <c r="K117" s="20">
+        <f t="shared" ref="K117:K119" si="20">SUM(B117:J117)</f>
+        <v>79.583333333333343</v>
+      </c>
+      <c r="L117" s="9">
+        <f t="shared" si="19"/>
+        <v>3</v>
+      </c>
+      <c r="N117" s="9"/>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A118" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="B118" s="9">
+        <f>B108*C18</f>
+        <v>7.5</v>
+      </c>
+      <c r="C118" s="9">
+        <f>C108*C19</f>
+        <v>10</v>
+      </c>
+      <c r="D118" s="9">
+        <f>D108*C20</f>
+        <v>11.25</v>
+      </c>
+      <c r="E118" s="9">
+        <f>E108*C21</f>
+        <v>7.5</v>
+      </c>
+      <c r="F118" s="9">
+        <f>F108*C22</f>
+        <v>7.5</v>
+      </c>
+      <c r="G118" s="20">
+        <f>G108*C23</f>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="H118" s="9">
+        <f>H108*C24</f>
+        <v>5</v>
+      </c>
+      <c r="I118" s="9">
+        <f>I108*C25</f>
+        <v>5</v>
+      </c>
+      <c r="J118" s="9">
+        <f>J108*C26</f>
+        <v>15</v>
+      </c>
+      <c r="K118" s="20">
+        <f t="shared" si="20"/>
+        <v>72.083333333333343</v>
+      </c>
+      <c r="L118" s="9">
+        <f>RANK(K118, $K$114:$K$119, 0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A119" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="B119" s="9">
+        <f>B109*C18</f>
+        <v>5</v>
+      </c>
+      <c r="C119" s="9">
+        <f>C109*19</f>
+        <v>9.5</v>
+      </c>
+      <c r="D119" s="9">
+        <f>D109*C20</f>
+        <v>11.25</v>
+      </c>
+      <c r="E119" s="9">
+        <f>E109*C21</f>
+        <v>7.5</v>
+      </c>
+      <c r="F119" s="9">
+        <f>F109*C22</f>
+        <v>10</v>
+      </c>
+      <c r="G119" s="20">
+        <f>G109*C23</f>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="H119" s="9">
+        <f>H109*C24</f>
+        <v>5</v>
+      </c>
+      <c r="I119" s="9">
+        <f>I109*C25</f>
+        <v>5</v>
+      </c>
+      <c r="J119" s="9">
+        <f>J109*C26</f>
+        <v>15</v>
+      </c>
+      <c r="K119" s="20">
+        <f t="shared" si="20"/>
+        <v>71.583333333333343</v>
+      </c>
+      <c r="L119" s="9">
+        <f t="shared" si="19"/>
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="L49">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L50">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A9D8EC-B5A1-466A-BFA2-9907A5A3DDF1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BDD87DC-8644-42C8-A7E5-56F463ADE935}">
   <dimension ref="A1:U112"/>
   <sheetViews>
@@ -6590,4 +9409,274 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1EACA8-BD40-42FD-A8BA-50E7DE06EFB6}">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="85" workbookViewId="0">
+      <selection sqref="A1:K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="23.88671875" customWidth="1"/>
+    <col min="7" max="7" width="19.21875" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" customWidth="1"/>
+    <col min="10" max="10" width="21.21875" customWidth="1"/>
+    <col min="11" max="11" width="26.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
revisi di pembinbing 1
</commit_message>
<xml_diff>
--- a/STUDI KASUS.xlsx
+++ b/STUDI KASUS.xlsx
@@ -5,22 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNDIPA\Semester 7\Skripsi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNDIPA\Semester 7\Skripsi\Format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D88FB68-8296-4CFF-9E7A-02A65EC74E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4A5CAB-1D26-425E-82F5-4EA45B0BB698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="691" xr2:uid="{901D0503-6946-40CA-8D36-37B156763246}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="691" activeTab="1" xr2:uid="{901D0503-6946-40CA-8D36-37B156763246}"/>
   </bookViews>
   <sheets>
     <sheet name="Kost" sheetId="3" r:id="rId1"/>
-    <sheet name="Ressponden" sheetId="1" r:id="rId2"/>
-    <sheet name="Bobot Kriteria" sheetId="2" r:id="rId3"/>
-    <sheet name="Studi Kasus for me" sheetId="4" r:id="rId4"/>
-    <sheet name="Studi Kasus for jurnal" sheetId="8" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
-    <sheet name="Hasil Bab 4" sheetId="6" r:id="rId7"/>
-    <sheet name="tumbal" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet2" sheetId="10" r:id="rId2"/>
+    <sheet name="Ressponden" sheetId="1" r:id="rId3"/>
+    <sheet name="Bobot Kriteria" sheetId="2" r:id="rId4"/>
+    <sheet name="Studi Kasus for me" sheetId="4" r:id="rId5"/>
+    <sheet name="Studi Kasus for jurnal" sheetId="8" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
+    <sheet name="Hasil Bab 4" sheetId="6" r:id="rId8"/>
+    <sheet name="tumbal" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="328">
   <si>
     <t xml:space="preserve">Biaya </t>
   </si>
@@ -997,12 +998,51 @@
   <si>
     <t>Jalan Sahabat 1 no 17</t>
   </si>
+  <si>
+    <t>Metode / Asumsi</t>
+  </si>
+  <si>
+    <t>Hasil sampel (pembulatan umum)</t>
+  </si>
+  <si>
+    <t>Slovin (e=0{,}05)</t>
+  </si>
+  <si>
+    <t>Slovin (e=0{,}10)</t>
+  </si>
+  <si>
+    <t>Cochran (adjusted, e=0{,}05, Z=1{,}96, p=0{,}5)</t>
+  </si>
+  <si>
+    <t>Cochran (adjusted, e=0{,}10)</t>
+  </si>
+  <si>
+    <t>Krejcie &amp; Morgan (tabel)</t>
+  </si>
+  <si>
+    <t>Isaac &amp; Michael (tabel)</t>
+  </si>
+  <si>
+    <t>Stratified (proporsional)</t>
+  </si>
+  <si>
+    <t>Cluster (two-stage)</t>
+  </si>
+  <si>
+    <t>Rumus</t>
+  </si>
+  <si>
+    <t>n=1+Ne2N​</t>
+  </si>
+  <si>
+    <t>n0​=e2Z2p(1−p)​</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1018,6 +1058,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1051,7 +1099,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1119,6 +1167,15 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2124,7 +2181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E46AEE5-C1DF-4E3B-B1A0-CC373A6F6C73}">
   <dimension ref="A2:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
+    <sheetView zoomScale="80" workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
@@ -2548,6 +2605,107 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EF27139-216E-4DDF-8D29-4F55B338C4CC}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.21875" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>315</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="B2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2" s="26">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="B3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C3" s="26">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="C4" s="26">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="C5" s="26">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="C6" s="26">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="C7" s="26">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="C8" s="28">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="C9" s="28">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7917028-436B-4FE2-9CD4-951DC7160D43}">
   <dimension ref="A1:N25"/>
   <sheetViews>
@@ -3093,7 +3251,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB87EEF9-7F2E-4545-9951-0F532151B120}">
   <dimension ref="A1:U27"/>
   <sheetViews>
@@ -3825,7 +3983,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BA1C62-8752-4999-BB16-F79297149C3E}">
   <dimension ref="A1:V112"/>
   <sheetViews>
@@ -5828,7 +5986,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6626FB-65A5-4DCB-9E1D-A2FA0EB2B8E1}">
   <dimension ref="A1:T119"/>
   <sheetViews>
@@ -8923,7 +9081,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A9D8EC-B5A1-466A-BFA2-9907A5A3DDF1}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -8935,7 +9093,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BDD87DC-8644-42C8-A7E5-56F463ADE935}">
   <dimension ref="A1:U112"/>
   <sheetViews>
@@ -10677,7 +10835,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1EACA8-BD40-42FD-A8BA-50E7DE06EFB6}">
   <dimension ref="A1:K7"/>
   <sheetViews>

</xml_diff>